<commit_message>
remove two nodes (food and feces), 2 arrows related to these nodes and update all the functions related to this modification
</commit_message>
<xml_diff>
--- a/todolist.xlsx
+++ b/todolist.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28702"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300"/>
   </bookViews>
   <sheets>
     <sheet name="To-Do List" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="32">
   <si>
     <t>Task</t>
   </si>
@@ -90,9 +90,6 @@
     <t>TO-DO LIST SPECIFIC TASKS</t>
   </si>
   <si>
-    <t>Asap</t>
-  </si>
-  <si>
     <t>update cases tudies app with the new design</t>
   </si>
   <si>
@@ -124,6 +121,15 @@
   </si>
   <si>
     <t>write base case with dashed line</t>
+  </si>
+  <si>
+    <t>Meeting planed in Lausanne</t>
+  </si>
+  <si>
+    <t>See with Olivier</t>
+  </si>
+  <si>
+    <t>see with Tara</t>
   </si>
 </sst>
 </file>
@@ -316,11 +322,11 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="11" applyFont="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="11" applyFont="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -559,7 +565,7 @@
         <xdr:cNvPr id="4" name="To Do Year" descr="Tab marker for year">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -625,7 +631,7 @@
         <xdr:cNvPr id="3" name="To Do Year" descr="Cell fill shape ">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -694,7 +700,7 @@
         <xdr:cNvPr id="7" name="To Do Year" descr="Tab marker for year">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -760,7 +766,7 @@
         <xdr:cNvPr id="8" name="To Do Year" descr="Cell fill shape ">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -834,7 +840,7 @@
         <xdr:cNvPr id="2" name="To Do Year" descr="Tab marker for year">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -905,7 +911,7 @@
         <xdr:cNvPr id="2" name="To Do Year" descr="Tab marker for year">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1355,8 +1361,8 @@
   </sheetPr>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1382,16 +1388,16 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
@@ -1427,7 +1433,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1">
         <f ca="1">DATE(Calendar_Year, 9, 12)</f>
@@ -1437,7 +1443,7 @@
         <v>43081</v>
       </c>
       <c r="G4" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H4" s="4">
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),-1,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),0,-1)))</f>
@@ -1454,8 +1460,8 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>18</v>
+      <c r="E5" s="6">
+        <v>43003</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="3">
@@ -1465,6 +1471,9 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),-1,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),0,-1)))</f>
         <v>-1</v>
       </c>
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
@@ -1488,6 +1497,9 @@
       <c r="H6" s="4">
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),-1,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),0,-1)))</f>
         <v>-1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -1563,7 +1575,7 @@
     </row>
     <row r="11" spans="1:9" ht="53" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -1581,7 +1593,7 @@
     </row>
     <row r="12" spans="1:9" ht="52" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -1599,7 +1611,7 @@
     </row>
     <row r="13" spans="1:9" ht="55" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -1614,10 +1626,13 @@
         <f ca="1">IF(AND(ToDoList3[[#This Row],[Status ]]="Complete",ToDoList3[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList3[[#This Row],[Due Date ]]),-1,IF(AND(ToDoList3[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList3[[#This Row],[Due Date ]]),0,-1)))</f>
         <v>-1</v>
       </c>
+      <c r="I13" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -1633,7 +1648,7 @@
         <v>-1</v>
       </c>
       <c r="I14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1780,7 +1795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1808,7 +1823,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="42" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1836,7 +1851,7 @@
     </row>
     <row r="3" spans="1:8" ht="42" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -1854,13 +1869,13 @@
     </row>
     <row r="4" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1874,7 +1889,7 @@
     </row>
     <row r="5" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2014,7 +2029,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="42" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2042,7 +2057,7 @@
     </row>
     <row r="3" spans="1:8" ht="42" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -2051,7 +2066,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>

</xml_diff>

<commit_message>
finish PHP1 notif improvement (case_study_app_V3)
</commit_message>
<xml_diff>
--- a/todolist.xlsx
+++ b/todolist.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300"/>
+    <workbookView xWindow="340" yWindow="-19580" windowWidth="28800" windowHeight="16300"/>
   </bookViews>
   <sheets>
     <sheet name="To-Do List" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="37">
   <si>
     <t>Task</t>
   </si>
@@ -117,9 +117,6 @@
     <t>color code inside sliders</t>
   </si>
   <si>
-    <t>ask with shiny developpers</t>
-  </si>
-  <si>
     <t>write base case with dashed line</t>
   </si>
   <si>
@@ -129,10 +126,25 @@
     <t>See with Olivier</t>
   </si>
   <si>
-    <t>see with Tara</t>
-  </si>
-  <si>
     <t>Complete</t>
+  </si>
+  <si>
+    <t>Deferred</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Not necessary at this time</t>
+  </si>
+  <si>
+    <t>Canceled</t>
+  </si>
+  <si>
+    <t>When the design is frozen</t>
   </si>
 </sst>
 </file>
@@ -568,7 +580,7 @@
         <xdr:cNvPr id="4" name="To Do Year" descr="Tab marker for year">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -634,7 +646,7 @@
         <xdr:cNvPr id="3" name="To Do Year" descr="Cell fill shape ">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -703,7 +715,7 @@
         <xdr:cNvPr id="7" name="To Do Year" descr="Tab marker for year">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -769,7 +781,7 @@
         <xdr:cNvPr id="8" name="To Do Year" descr="Cell fill shape ">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -843,7 +855,7 @@
         <xdr:cNvPr id="2" name="To Do Year" descr="Tab marker for year">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -914,7 +926,7 @@
         <xdr:cNvPr id="2" name="To Do Year" descr="Tab marker for year">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1365,7 +1377,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1446,7 +1458,7 @@
         <v>43081</v>
       </c>
       <c r="G4" s="3">
-        <v>0.1</v>
+        <v>0.75</v>
       </c>
       <c r="H4" s="4">
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),-1,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),0,-1)))</f>
@@ -1461,7 +1473,7 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E5" s="6">
         <v>43003</v>
@@ -1475,7 +1487,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -1495,14 +1507,14 @@
         <v>43160</v>
       </c>
       <c r="G6" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H6" s="4">
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),-1,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),0,-1)))</f>
         <v>-1</v>
       </c>
       <c r="I6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -1527,6 +1539,9 @@
       <c r="H7" s="4">
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),-1,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),0,-1)))</f>
         <v>-1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -1584,14 +1599,16 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
       <c r="H11" s="4">
         <f ca="1">IF(AND(ToDoList3[[#This Row],[Status ]]="Complete",ToDoList3[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList3[[#This Row],[Due Date ]]),-1,IF(AND(ToDoList3[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList3[[#This Row],[Due Date ]]),0,-1)))</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="52" customHeight="1" x14ac:dyDescent="0.15">
@@ -1611,6 +1628,9 @@
         <f ca="1">IF(AND(ToDoList3[[#This Row],[Status ]]="Complete",ToDoList3[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList3[[#This Row],[Due Date ]]),-1,IF(AND(ToDoList3[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList3[[#This Row],[Due Date ]]),0,-1)))</f>
         <v>-1</v>
       </c>
+      <c r="I12" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="55" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
@@ -1620,7 +1640,7 @@
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1630,7 +1650,7 @@
         <v>-1</v>
       </c>
       <c r="I13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.15">
@@ -1641,17 +1661,19 @@
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="3"/>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
       <c r="H14" s="4">
         <f ca="1">IF(AND(ToDoList3[[#This Row],[Status ]]="Complete",ToDoList3[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList3[[#This Row],[Due Date ]]),-1,IF(AND(ToDoList3[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList3[[#This Row],[Due Date ]]),0,-1)))</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1799,7 +1821,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1860,11 +1882,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3">
+        <v>0.5</v>
+      </c>
       <c r="G3" s="4">
         <f ca="1">IF(AND(ToDoList32[[#This Row],[Status ]]="Complete",ToDoList32[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList32[[#This Row],[Due Date ]]),-1,IF(AND(ToDoList32[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList32[[#This Row],[Due Date ]]),0,-1)))</f>
         <v>-1</v>
@@ -1878,21 +1902,22 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="3">
-        <v>0.5</v>
-      </c>
+      <c r="F4" s="3"/>
       <c r="G4" s="4">
         <f ca="1">IF(AND(ToDoList32[[#This Row],[Status ]]="Complete",ToDoList32[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList32[[#This Row],[Due Date ]]),-1,IF(AND(ToDoList32[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList32[[#This Row],[Due Date ]]),0,-1)))</f>
         <v>-1</v>
       </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2005,7 +2030,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2062,6 +2087,12 @@
       <c r="A3" t="s">
         <v>24</v>
       </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="3"/>
@@ -2070,6 +2101,12 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>

</xml_diff>